<commit_message>
Updates:  - test data files  - test spreadsheet  - gitignore changes
</commit_message>
<xml_diff>
--- a/UnitTests/Test_Matrix.xlsx
+++ b/UnitTests/Test_Matrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="73">
   <si>
     <t>File Name</t>
   </si>
@@ -218,6 +218,27 @@
   </si>
   <si>
     <t>Test_003</t>
+  </si>
+  <si>
+    <t>Test_004</t>
+  </si>
+  <si>
+    <t>Effective Addresssing</t>
+  </si>
+  <si>
+    <t>ILLEGAL</t>
+  </si>
+  <si>
+    <t>NOP</t>
+  </si>
+  <si>
+    <t>SUBQ.B</t>
+  </si>
+  <si>
+    <t>SUBQ.W</t>
+  </si>
+  <si>
+    <t>SUBQ.L</t>
   </si>
 </sst>
 </file>
@@ -233,15 +254,33 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="21">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -477,11 +516,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
@@ -539,18 +593,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -585,6 +627,57 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -867,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AT50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AK6" sqref="AK6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,57 +975,57 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="28" t="s">
+      <c r="C1" s="63"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="28"/>
-      <c r="Z1" s="28"/>
-      <c r="AA1" s="28"/>
-      <c r="AB1" s="28"/>
-      <c r="AC1" s="28"/>
-      <c r="AD1" s="28"/>
-      <c r="AE1" s="28"/>
-      <c r="AF1" s="28"/>
-      <c r="AG1" s="28"/>
-      <c r="AH1" s="28"/>
-      <c r="AI1" s="28"/>
-      <c r="AJ1" s="28"/>
-      <c r="AK1" s="28"/>
-      <c r="AL1" s="28"/>
-      <c r="AM1" s="28" t="s">
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="65"/>
+      <c r="N1" s="65"/>
+      <c r="O1" s="65"/>
+      <c r="P1" s="65"/>
+      <c r="Q1" s="65"/>
+      <c r="R1" s="65"/>
+      <c r="S1" s="65"/>
+      <c r="T1" s="65"/>
+      <c r="U1" s="65"/>
+      <c r="V1" s="65"/>
+      <c r="W1" s="65"/>
+      <c r="X1" s="65"/>
+      <c r="Y1" s="65"/>
+      <c r="Z1" s="65"/>
+      <c r="AA1" s="65"/>
+      <c r="AB1" s="65"/>
+      <c r="AC1" s="65"/>
+      <c r="AD1" s="65"/>
+      <c r="AE1" s="65"/>
+      <c r="AF1" s="65"/>
+      <c r="AG1" s="65"/>
+      <c r="AH1" s="65"/>
+      <c r="AI1" s="65"/>
+      <c r="AJ1" s="65"/>
+      <c r="AK1" s="65"/>
+      <c r="AL1" s="65"/>
+      <c r="AM1" s="65" t="s">
         <v>56</v>
       </c>
-      <c r="AN1" s="28"/>
-      <c r="AO1" s="28"/>
-      <c r="AP1" s="28"/>
-      <c r="AQ1" s="28"/>
-      <c r="AR1" s="28"/>
-      <c r="AS1" s="28"/>
-      <c r="AT1" s="28"/>
+      <c r="AN1" s="65"/>
+      <c r="AO1" s="65"/>
+      <c r="AP1" s="65"/>
+      <c r="AQ1" s="65"/>
+      <c r="AR1" s="65"/>
+      <c r="AS1" s="65"/>
+      <c r="AT1" s="65"/>
     </row>
     <row r="2" spans="1:46" s="2" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
       <c r="B2" s="19"/>
@@ -1040,14 +1133,14 @@
       <c r="AL2" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="AM2" s="36"/>
-      <c r="AN2" s="37"/>
-      <c r="AO2" s="37"/>
-      <c r="AP2" s="37"/>
-      <c r="AQ2" s="37"/>
-      <c r="AR2" s="37"/>
-      <c r="AS2" s="37"/>
-      <c r="AT2" s="38"/>
+      <c r="AM2" s="32"/>
+      <c r="AN2" s="33"/>
+      <c r="AO2" s="33"/>
+      <c r="AP2" s="33"/>
+      <c r="AQ2" s="33"/>
+      <c r="AR2" s="33"/>
+      <c r="AS2" s="33"/>
+      <c r="AT2" s="34"/>
     </row>
     <row r="3" spans="1:46" s="1" customFormat="1" ht="53.25" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
@@ -1161,28 +1254,28 @@
       <c r="AL3" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="AM3" s="39" t="s">
+      <c r="AM3" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="AN3" s="40" t="s">
+      <c r="AN3" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="AO3" s="40" t="s">
+      <c r="AO3" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="AP3" s="40" t="s">
+      <c r="AP3" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="AQ3" s="41" t="s">
+      <c r="AQ3" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="AR3" s="41" t="s">
+      <c r="AR3" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="AS3" s="40" t="s">
+      <c r="AS3" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="AT3" s="42" t="s">
+      <c r="AT3" s="38" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1233,146 +1326,88 @@
       <c r="AJ4" s="10"/>
       <c r="AK4" s="10"/>
       <c r="AL4" s="11"/>
-      <c r="AM4" s="43"/>
-      <c r="AN4" s="44"/>
-      <c r="AO4" s="44"/>
-      <c r="AP4" s="44"/>
-      <c r="AQ4" s="44"/>
-      <c r="AR4" s="44"/>
-      <c r="AS4" s="44"/>
-      <c r="AT4" s="45"/>
+      <c r="AM4" s="39"/>
+      <c r="AN4" s="40"/>
+      <c r="AO4" s="40"/>
+      <c r="AP4" s="40"/>
+      <c r="AQ4" s="40"/>
+      <c r="AR4" s="40"/>
+      <c r="AS4" s="40"/>
+      <c r="AT4" s="41"/>
     </row>
     <row r="5" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="L5" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="M5" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="N5" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="O5" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="P5" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q5" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="R5" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="S5" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="T5" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="U5" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="V5" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="W5" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="X5" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="Y5" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="Z5" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA5" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="AB5" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="AC5" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AD5" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="AE5" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="AF5" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AG5" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="AH5" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="AI5" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="AJ5" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="AK5" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="AL5" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AM5" s="43"/>
-      <c r="AN5" s="44"/>
-      <c r="AO5" s="44"/>
-      <c r="AP5" s="44"/>
-      <c r="AQ5" s="44"/>
-      <c r="AR5" s="44"/>
-      <c r="AS5" s="44"/>
-      <c r="AT5" s="45"/>
+      <c r="B5" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="49"/>
+      <c r="J5" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="K5" s="49" t="s">
+        <v>5</v>
+      </c>
+      <c r="L5" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="M5" s="49" t="s">
+        <v>5</v>
+      </c>
+      <c r="N5" s="50"/>
+      <c r="O5" s="48"/>
+      <c r="P5" s="48"/>
+      <c r="Q5" s="48"/>
+      <c r="R5" s="49"/>
+      <c r="S5" s="51"/>
+      <c r="T5" s="50"/>
+      <c r="U5" s="48"/>
+      <c r="V5" s="48"/>
+      <c r="W5" s="48"/>
+      <c r="X5" s="49"/>
+      <c r="Y5" s="50"/>
+      <c r="Z5" s="49"/>
+      <c r="AA5" s="51"/>
+      <c r="AB5" s="50"/>
+      <c r="AC5" s="49"/>
+      <c r="AD5" s="51"/>
+      <c r="AE5" s="50"/>
+      <c r="AF5" s="49"/>
+      <c r="AG5" s="50"/>
+      <c r="AH5" s="48"/>
+      <c r="AI5" s="48"/>
+      <c r="AJ5" s="48"/>
+      <c r="AK5" s="48"/>
+      <c r="AL5" s="49"/>
+      <c r="AM5" s="52"/>
+      <c r="AN5" s="53"/>
+      <c r="AO5" s="53"/>
+      <c r="AP5" s="53"/>
+      <c r="AQ5" s="53"/>
+      <c r="AR5" s="53"/>
+      <c r="AS5" s="53"/>
+      <c r="AT5" s="54"/>
     </row>
     <row r="6" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="29"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="31"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="27"/>
       <c r="E6" s="10" t="s">
         <v>5</v>
       </c>
@@ -1413,35 +1448,50 @@
       <c r="AJ6" s="10"/>
       <c r="AK6" s="10"/>
       <c r="AL6" s="11"/>
-      <c r="AM6" s="43" t="s">
-        <v>5</v>
-      </c>
-      <c r="AN6" s="44"/>
-      <c r="AO6" s="44"/>
-      <c r="AP6" s="44"/>
-      <c r="AQ6" s="44"/>
-      <c r="AR6" s="44" t="s">
-        <v>5</v>
-      </c>
-      <c r="AS6" s="44"/>
-      <c r="AT6" s="45"/>
+      <c r="AM6" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN6" s="40"/>
+      <c r="AO6" s="40"/>
+      <c r="AP6" s="40"/>
+      <c r="AQ6" s="40"/>
+      <c r="AR6" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="AS6" s="40"/>
+      <c r="AT6" s="41"/>
     </row>
     <row r="7" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="B7" s="29"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="31"/>
+      <c r="A7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="25"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="27"/>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
       <c r="G7" s="11"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="11"/>
+      <c r="H7" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="M7" s="11" t="s">
+        <v>5</v>
+      </c>
       <c r="N7" s="9"/>
-      <c r="O7" s="35"/>
-      <c r="P7" s="35"/>
+      <c r="O7" s="31"/>
+      <c r="P7" s="31"/>
       <c r="Q7" s="10"/>
       <c r="R7" s="11"/>
       <c r="S7" s="17"/>
@@ -1464,19 +1514,35 @@
       <c r="AJ7" s="10"/>
       <c r="AK7" s="10"/>
       <c r="AL7" s="11"/>
-      <c r="AM7" s="43"/>
-      <c r="AN7" s="44"/>
-      <c r="AO7" s="44"/>
-      <c r="AP7" s="44"/>
-      <c r="AQ7" s="44"/>
-      <c r="AR7" s="44"/>
-      <c r="AS7" s="44"/>
-      <c r="AT7" s="45"/>
+      <c r="AM7" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN7" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="AO7" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP7" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="AQ7" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="AR7" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="AS7" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="AT7" s="41" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="B8" s="29"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="31"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="27"/>
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
       <c r="G8" s="11"/>
@@ -1511,19 +1577,19 @@
       <c r="AJ8" s="10"/>
       <c r="AK8" s="10"/>
       <c r="AL8" s="11"/>
-      <c r="AM8" s="43"/>
-      <c r="AN8" s="44"/>
-      <c r="AO8" s="44"/>
-      <c r="AP8" s="44"/>
-      <c r="AQ8" s="44"/>
-      <c r="AR8" s="44"/>
-      <c r="AS8" s="44"/>
-      <c r="AT8" s="45"/>
+      <c r="AM8" s="39"/>
+      <c r="AN8" s="40"/>
+      <c r="AO8" s="40"/>
+      <c r="AP8" s="40"/>
+      <c r="AQ8" s="40"/>
+      <c r="AR8" s="40"/>
+      <c r="AS8" s="40"/>
+      <c r="AT8" s="41"/>
     </row>
     <row r="9" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="B9" s="29"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="31"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="27"/>
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
       <c r="G9" s="11"/>
@@ -1558,19 +1624,19 @@
       <c r="AJ9" s="10"/>
       <c r="AK9" s="10"/>
       <c r="AL9" s="11"/>
-      <c r="AM9" s="43"/>
-      <c r="AN9" s="44"/>
-      <c r="AO9" s="44"/>
-      <c r="AP9" s="44"/>
-      <c r="AQ9" s="44"/>
-      <c r="AR9" s="44"/>
-      <c r="AS9" s="44"/>
-      <c r="AT9" s="45"/>
+      <c r="AM9" s="39"/>
+      <c r="AN9" s="40"/>
+      <c r="AO9" s="40"/>
+      <c r="AP9" s="40"/>
+      <c r="AQ9" s="40"/>
+      <c r="AR9" s="40"/>
+      <c r="AS9" s="40"/>
+      <c r="AT9" s="41"/>
     </row>
     <row r="10" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="B10" s="29"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="31"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="27"/>
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
       <c r="G10" s="11"/>
@@ -1605,19 +1671,19 @@
       <c r="AJ10" s="10"/>
       <c r="AK10" s="10"/>
       <c r="AL10" s="11"/>
-      <c r="AM10" s="43"/>
-      <c r="AN10" s="44"/>
-      <c r="AO10" s="44"/>
-      <c r="AP10" s="44"/>
-      <c r="AQ10" s="44"/>
-      <c r="AR10" s="44"/>
-      <c r="AS10" s="44"/>
-      <c r="AT10" s="45"/>
+      <c r="AM10" s="39"/>
+      <c r="AN10" s="40"/>
+      <c r="AO10" s="40"/>
+      <c r="AP10" s="40"/>
+      <c r="AQ10" s="40"/>
+      <c r="AR10" s="40"/>
+      <c r="AS10" s="40"/>
+      <c r="AT10" s="41"/>
     </row>
     <row r="11" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="B11" s="29"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="31"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="27"/>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
       <c r="G11" s="11"/>
@@ -1652,19 +1718,19 @@
       <c r="AJ11" s="10"/>
       <c r="AK11" s="10"/>
       <c r="AL11" s="11"/>
-      <c r="AM11" s="43"/>
-      <c r="AN11" s="44"/>
-      <c r="AO11" s="44"/>
-      <c r="AP11" s="44"/>
-      <c r="AQ11" s="44"/>
-      <c r="AR11" s="44"/>
-      <c r="AS11" s="44"/>
-      <c r="AT11" s="45"/>
+      <c r="AM11" s="39"/>
+      <c r="AN11" s="40"/>
+      <c r="AO11" s="40"/>
+      <c r="AP11" s="40"/>
+      <c r="AQ11" s="40"/>
+      <c r="AR11" s="40"/>
+      <c r="AS11" s="40"/>
+      <c r="AT11" s="41"/>
     </row>
     <row r="12" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="B12" s="29"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="31"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="27"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
       <c r="G12" s="11"/>
@@ -1699,19 +1765,19 @@
       <c r="AJ12" s="10"/>
       <c r="AK12" s="10"/>
       <c r="AL12" s="11"/>
-      <c r="AM12" s="43"/>
-      <c r="AN12" s="44"/>
-      <c r="AO12" s="44"/>
-      <c r="AP12" s="44"/>
-      <c r="AQ12" s="44"/>
-      <c r="AR12" s="44"/>
-      <c r="AS12" s="44"/>
-      <c r="AT12" s="45"/>
+      <c r="AM12" s="39"/>
+      <c r="AN12" s="40"/>
+      <c r="AO12" s="40"/>
+      <c r="AP12" s="40"/>
+      <c r="AQ12" s="40"/>
+      <c r="AR12" s="40"/>
+      <c r="AS12" s="40"/>
+      <c r="AT12" s="41"/>
     </row>
     <row r="13" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="B13" s="29"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="31"/>
+      <c r="B13" s="25"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="27"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
       <c r="G13" s="11"/>
@@ -1746,19 +1812,19 @@
       <c r="AJ13" s="10"/>
       <c r="AK13" s="10"/>
       <c r="AL13" s="11"/>
-      <c r="AM13" s="43"/>
-      <c r="AN13" s="44"/>
-      <c r="AO13" s="44"/>
-      <c r="AP13" s="44"/>
-      <c r="AQ13" s="44"/>
-      <c r="AR13" s="44"/>
-      <c r="AS13" s="44"/>
-      <c r="AT13" s="45"/>
+      <c r="AM13" s="39"/>
+      <c r="AN13" s="40"/>
+      <c r="AO13" s="40"/>
+      <c r="AP13" s="40"/>
+      <c r="AQ13" s="40"/>
+      <c r="AR13" s="40"/>
+      <c r="AS13" s="40"/>
+      <c r="AT13" s="41"/>
     </row>
     <row r="14" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="B14" s="29"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="31"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="27"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
       <c r="G14" s="11"/>
@@ -1793,19 +1859,19 @@
       <c r="AJ14" s="10"/>
       <c r="AK14" s="10"/>
       <c r="AL14" s="11"/>
-      <c r="AM14" s="43"/>
-      <c r="AN14" s="44"/>
-      <c r="AO14" s="44"/>
-      <c r="AP14" s="44"/>
-      <c r="AQ14" s="44"/>
-      <c r="AR14" s="44"/>
-      <c r="AS14" s="44"/>
-      <c r="AT14" s="45"/>
+      <c r="AM14" s="39"/>
+      <c r="AN14" s="40"/>
+      <c r="AO14" s="40"/>
+      <c r="AP14" s="40"/>
+      <c r="AQ14" s="40"/>
+      <c r="AR14" s="40"/>
+      <c r="AS14" s="40"/>
+      <c r="AT14" s="41"/>
     </row>
     <row r="15" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="B15" s="29"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="31"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="27"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
       <c r="G15" s="11"/>
@@ -1840,19 +1906,19 @@
       <c r="AJ15" s="10"/>
       <c r="AK15" s="10"/>
       <c r="AL15" s="11"/>
-      <c r="AM15" s="43"/>
-      <c r="AN15" s="44"/>
-      <c r="AO15" s="44"/>
-      <c r="AP15" s="44"/>
-      <c r="AQ15" s="44"/>
-      <c r="AR15" s="44"/>
-      <c r="AS15" s="44"/>
-      <c r="AT15" s="45"/>
+      <c r="AM15" s="39"/>
+      <c r="AN15" s="40"/>
+      <c r="AO15" s="40"/>
+      <c r="AP15" s="40"/>
+      <c r="AQ15" s="40"/>
+      <c r="AR15" s="40"/>
+      <c r="AS15" s="40"/>
+      <c r="AT15" s="41"/>
     </row>
     <row r="16" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="B16" s="29"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="31"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="27"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="11"/>
@@ -1887,19 +1953,19 @@
       <c r="AJ16" s="10"/>
       <c r="AK16" s="10"/>
       <c r="AL16" s="11"/>
-      <c r="AM16" s="43"/>
-      <c r="AN16" s="44"/>
-      <c r="AO16" s="44"/>
-      <c r="AP16" s="44"/>
-      <c r="AQ16" s="44"/>
-      <c r="AR16" s="44"/>
-      <c r="AS16" s="44"/>
-      <c r="AT16" s="45"/>
+      <c r="AM16" s="39"/>
+      <c r="AN16" s="40"/>
+      <c r="AO16" s="40"/>
+      <c r="AP16" s="40"/>
+      <c r="AQ16" s="40"/>
+      <c r="AR16" s="40"/>
+      <c r="AS16" s="40"/>
+      <c r="AT16" s="41"/>
     </row>
     <row r="17" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B17" s="29"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="31"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="27"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="11"/>
@@ -1934,19 +2000,19 @@
       <c r="AJ17" s="10"/>
       <c r="AK17" s="10"/>
       <c r="AL17" s="11"/>
-      <c r="AM17" s="43"/>
-      <c r="AN17" s="44"/>
-      <c r="AO17" s="44"/>
-      <c r="AP17" s="44"/>
-      <c r="AQ17" s="44"/>
-      <c r="AR17" s="44"/>
-      <c r="AS17" s="44"/>
-      <c r="AT17" s="45"/>
+      <c r="AM17" s="39"/>
+      <c r="AN17" s="40"/>
+      <c r="AO17" s="40"/>
+      <c r="AP17" s="40"/>
+      <c r="AQ17" s="40"/>
+      <c r="AR17" s="40"/>
+      <c r="AS17" s="40"/>
+      <c r="AT17" s="41"/>
     </row>
     <row r="18" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B18" s="29"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="31"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="27"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="11"/>
@@ -1981,19 +2047,19 @@
       <c r="AJ18" s="10"/>
       <c r="AK18" s="10"/>
       <c r="AL18" s="11"/>
-      <c r="AM18" s="43"/>
-      <c r="AN18" s="44"/>
-      <c r="AO18" s="44"/>
-      <c r="AP18" s="44"/>
-      <c r="AQ18" s="44"/>
-      <c r="AR18" s="44"/>
-      <c r="AS18" s="44"/>
-      <c r="AT18" s="45"/>
+      <c r="AM18" s="39"/>
+      <c r="AN18" s="40"/>
+      <c r="AO18" s="40"/>
+      <c r="AP18" s="40"/>
+      <c r="AQ18" s="40"/>
+      <c r="AR18" s="40"/>
+      <c r="AS18" s="40"/>
+      <c r="AT18" s="41"/>
     </row>
     <row r="19" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B19" s="29"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="31"/>
+      <c r="B19" s="25"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="27"/>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
       <c r="G19" s="11"/>
@@ -2028,19 +2094,19 @@
       <c r="AJ19" s="10"/>
       <c r="AK19" s="10"/>
       <c r="AL19" s="11"/>
-      <c r="AM19" s="43"/>
-      <c r="AN19" s="44"/>
-      <c r="AO19" s="44"/>
-      <c r="AP19" s="44"/>
-      <c r="AQ19" s="44"/>
-      <c r="AR19" s="44"/>
-      <c r="AS19" s="44"/>
-      <c r="AT19" s="45"/>
+      <c r="AM19" s="39"/>
+      <c r="AN19" s="40"/>
+      <c r="AO19" s="40"/>
+      <c r="AP19" s="40"/>
+      <c r="AQ19" s="40"/>
+      <c r="AR19" s="40"/>
+      <c r="AS19" s="40"/>
+      <c r="AT19" s="41"/>
     </row>
     <row r="20" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B20" s="29"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="31"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="27"/>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
       <c r="G20" s="11"/>
@@ -2075,19 +2141,19 @@
       <c r="AJ20" s="10"/>
       <c r="AK20" s="10"/>
       <c r="AL20" s="11"/>
-      <c r="AM20" s="43"/>
-      <c r="AN20" s="44"/>
-      <c r="AO20" s="44"/>
-      <c r="AP20" s="44"/>
-      <c r="AQ20" s="44"/>
-      <c r="AR20" s="44"/>
-      <c r="AS20" s="44"/>
-      <c r="AT20" s="45"/>
+      <c r="AM20" s="39"/>
+      <c r="AN20" s="40"/>
+      <c r="AO20" s="40"/>
+      <c r="AP20" s="40"/>
+      <c r="AQ20" s="40"/>
+      <c r="AR20" s="40"/>
+      <c r="AS20" s="40"/>
+      <c r="AT20" s="41"/>
     </row>
     <row r="21" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B21" s="29"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="31"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="27"/>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
       <c r="G21" s="11"/>
@@ -2122,19 +2188,19 @@
       <c r="AJ21" s="10"/>
       <c r="AK21" s="10"/>
       <c r="AL21" s="11"/>
-      <c r="AM21" s="43"/>
-      <c r="AN21" s="44"/>
-      <c r="AO21" s="44"/>
-      <c r="AP21" s="44"/>
-      <c r="AQ21" s="44"/>
-      <c r="AR21" s="44"/>
-      <c r="AS21" s="44"/>
-      <c r="AT21" s="45"/>
+      <c r="AM21" s="39"/>
+      <c r="AN21" s="40"/>
+      <c r="AO21" s="40"/>
+      <c r="AP21" s="40"/>
+      <c r="AQ21" s="40"/>
+      <c r="AR21" s="40"/>
+      <c r="AS21" s="40"/>
+      <c r="AT21" s="41"/>
     </row>
     <row r="22" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B22" s="29"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="31"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="27"/>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
       <c r="G22" s="11"/>
@@ -2169,19 +2235,19 @@
       <c r="AJ22" s="10"/>
       <c r="AK22" s="10"/>
       <c r="AL22" s="11"/>
-      <c r="AM22" s="43"/>
-      <c r="AN22" s="44"/>
-      <c r="AO22" s="44"/>
-      <c r="AP22" s="44"/>
-      <c r="AQ22" s="44"/>
-      <c r="AR22" s="44"/>
-      <c r="AS22" s="44"/>
-      <c r="AT22" s="45"/>
+      <c r="AM22" s="39"/>
+      <c r="AN22" s="40"/>
+      <c r="AO22" s="40"/>
+      <c r="AP22" s="40"/>
+      <c r="AQ22" s="40"/>
+      <c r="AR22" s="40"/>
+      <c r="AS22" s="40"/>
+      <c r="AT22" s="41"/>
     </row>
     <row r="23" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B23" s="29"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="31"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="27"/>
       <c r="E23" s="10"/>
       <c r="F23" s="10"/>
       <c r="G23" s="11"/>
@@ -2216,19 +2282,19 @@
       <c r="AJ23" s="10"/>
       <c r="AK23" s="10"/>
       <c r="AL23" s="11"/>
-      <c r="AM23" s="43"/>
-      <c r="AN23" s="44"/>
-      <c r="AO23" s="44"/>
-      <c r="AP23" s="44"/>
-      <c r="AQ23" s="44"/>
-      <c r="AR23" s="44"/>
-      <c r="AS23" s="44"/>
-      <c r="AT23" s="45"/>
+      <c r="AM23" s="39"/>
+      <c r="AN23" s="40"/>
+      <c r="AO23" s="40"/>
+      <c r="AP23" s="40"/>
+      <c r="AQ23" s="40"/>
+      <c r="AR23" s="40"/>
+      <c r="AS23" s="40"/>
+      <c r="AT23" s="41"/>
     </row>
     <row r="24" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B24" s="29"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="31"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="27"/>
       <c r="E24" s="10"/>
       <c r="F24" s="10"/>
       <c r="G24" s="11"/>
@@ -2263,19 +2329,19 @@
       <c r="AJ24" s="10"/>
       <c r="AK24" s="10"/>
       <c r="AL24" s="11"/>
-      <c r="AM24" s="43"/>
-      <c r="AN24" s="44"/>
-      <c r="AO24" s="44"/>
-      <c r="AP24" s="44"/>
-      <c r="AQ24" s="44"/>
-      <c r="AR24" s="44"/>
-      <c r="AS24" s="44"/>
-      <c r="AT24" s="45"/>
+      <c r="AM24" s="39"/>
+      <c r="AN24" s="40"/>
+      <c r="AO24" s="40"/>
+      <c r="AP24" s="40"/>
+      <c r="AQ24" s="40"/>
+      <c r="AR24" s="40"/>
+      <c r="AS24" s="40"/>
+      <c r="AT24" s="41"/>
     </row>
     <row r="25" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B25" s="29"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="31"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="27"/>
       <c r="E25" s="10"/>
       <c r="F25" s="10"/>
       <c r="G25" s="11"/>
@@ -2310,19 +2376,19 @@
       <c r="AJ25" s="10"/>
       <c r="AK25" s="10"/>
       <c r="AL25" s="11"/>
-      <c r="AM25" s="43"/>
-      <c r="AN25" s="44"/>
-      <c r="AO25" s="44"/>
-      <c r="AP25" s="44"/>
-      <c r="AQ25" s="44"/>
-      <c r="AR25" s="44"/>
-      <c r="AS25" s="44"/>
-      <c r="AT25" s="45"/>
+      <c r="AM25" s="39"/>
+      <c r="AN25" s="40"/>
+      <c r="AO25" s="40"/>
+      <c r="AP25" s="40"/>
+      <c r="AQ25" s="40"/>
+      <c r="AR25" s="40"/>
+      <c r="AS25" s="40"/>
+      <c r="AT25" s="41"/>
     </row>
     <row r="26" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B26" s="29"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="31"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="27"/>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
       <c r="G26" s="11"/>
@@ -2357,19 +2423,19 @@
       <c r="AJ26" s="10"/>
       <c r="AK26" s="10"/>
       <c r="AL26" s="11"/>
-      <c r="AM26" s="43"/>
-      <c r="AN26" s="44"/>
-      <c r="AO26" s="44"/>
-      <c r="AP26" s="44"/>
-      <c r="AQ26" s="44"/>
-      <c r="AR26" s="44"/>
-      <c r="AS26" s="44"/>
-      <c r="AT26" s="45"/>
+      <c r="AM26" s="39"/>
+      <c r="AN26" s="40"/>
+      <c r="AO26" s="40"/>
+      <c r="AP26" s="40"/>
+      <c r="AQ26" s="40"/>
+      <c r="AR26" s="40"/>
+      <c r="AS26" s="40"/>
+      <c r="AT26" s="41"/>
     </row>
     <row r="27" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B27" s="29"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="31"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="27"/>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
       <c r="G27" s="11"/>
@@ -2404,19 +2470,19 @@
       <c r="AJ27" s="10"/>
       <c r="AK27" s="10"/>
       <c r="AL27" s="11"/>
-      <c r="AM27" s="43"/>
-      <c r="AN27" s="44"/>
-      <c r="AO27" s="44"/>
-      <c r="AP27" s="44"/>
-      <c r="AQ27" s="44"/>
-      <c r="AR27" s="44"/>
-      <c r="AS27" s="44"/>
-      <c r="AT27" s="45"/>
+      <c r="AM27" s="39"/>
+      <c r="AN27" s="40"/>
+      <c r="AO27" s="40"/>
+      <c r="AP27" s="40"/>
+      <c r="AQ27" s="40"/>
+      <c r="AR27" s="40"/>
+      <c r="AS27" s="40"/>
+      <c r="AT27" s="41"/>
     </row>
     <row r="28" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B28" s="29"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="31"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="27"/>
       <c r="E28" s="10"/>
       <c r="F28" s="10"/>
       <c r="G28" s="11"/>
@@ -2451,19 +2517,19 @@
       <c r="AJ28" s="10"/>
       <c r="AK28" s="10"/>
       <c r="AL28" s="11"/>
-      <c r="AM28" s="43"/>
-      <c r="AN28" s="44"/>
-      <c r="AO28" s="44"/>
-      <c r="AP28" s="44"/>
-      <c r="AQ28" s="44"/>
-      <c r="AR28" s="44"/>
-      <c r="AS28" s="44"/>
-      <c r="AT28" s="45"/>
+      <c r="AM28" s="39"/>
+      <c r="AN28" s="40"/>
+      <c r="AO28" s="40"/>
+      <c r="AP28" s="40"/>
+      <c r="AQ28" s="40"/>
+      <c r="AR28" s="40"/>
+      <c r="AS28" s="40"/>
+      <c r="AT28" s="41"/>
     </row>
     <row r="29" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B29" s="29"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="31"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="27"/>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
       <c r="G29" s="11"/>
@@ -2498,19 +2564,19 @@
       <c r="AJ29" s="10"/>
       <c r="AK29" s="10"/>
       <c r="AL29" s="11"/>
-      <c r="AM29" s="43"/>
-      <c r="AN29" s="44"/>
-      <c r="AO29" s="44"/>
-      <c r="AP29" s="44"/>
-      <c r="AQ29" s="44"/>
-      <c r="AR29" s="44"/>
-      <c r="AS29" s="44"/>
-      <c r="AT29" s="45"/>
+      <c r="AM29" s="39"/>
+      <c r="AN29" s="40"/>
+      <c r="AO29" s="40"/>
+      <c r="AP29" s="40"/>
+      <c r="AQ29" s="40"/>
+      <c r="AR29" s="40"/>
+      <c r="AS29" s="40"/>
+      <c r="AT29" s="41"/>
     </row>
     <row r="30" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B30" s="29"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="31"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="27"/>
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
       <c r="G30" s="11"/>
@@ -2545,19 +2611,19 @@
       <c r="AJ30" s="10"/>
       <c r="AK30" s="10"/>
       <c r="AL30" s="11"/>
-      <c r="AM30" s="43"/>
-      <c r="AN30" s="44"/>
-      <c r="AO30" s="44"/>
-      <c r="AP30" s="44"/>
-      <c r="AQ30" s="44"/>
-      <c r="AR30" s="44"/>
-      <c r="AS30" s="44"/>
-      <c r="AT30" s="45"/>
+      <c r="AM30" s="39"/>
+      <c r="AN30" s="40"/>
+      <c r="AO30" s="40"/>
+      <c r="AP30" s="40"/>
+      <c r="AQ30" s="40"/>
+      <c r="AR30" s="40"/>
+      <c r="AS30" s="40"/>
+      <c r="AT30" s="41"/>
     </row>
     <row r="31" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B31" s="29"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="31"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="27"/>
       <c r="E31" s="10"/>
       <c r="F31" s="10"/>
       <c r="G31" s="11"/>
@@ -2592,19 +2658,19 @@
       <c r="AJ31" s="10"/>
       <c r="AK31" s="10"/>
       <c r="AL31" s="11"/>
-      <c r="AM31" s="43"/>
-      <c r="AN31" s="44"/>
-      <c r="AO31" s="44"/>
-      <c r="AP31" s="44"/>
-      <c r="AQ31" s="44"/>
-      <c r="AR31" s="44"/>
-      <c r="AS31" s="44"/>
-      <c r="AT31" s="45"/>
+      <c r="AM31" s="39"/>
+      <c r="AN31" s="40"/>
+      <c r="AO31" s="40"/>
+      <c r="AP31" s="40"/>
+      <c r="AQ31" s="40"/>
+      <c r="AR31" s="40"/>
+      <c r="AS31" s="40"/>
+      <c r="AT31" s="41"/>
     </row>
     <row r="32" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B32" s="29"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="31"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="27"/>
       <c r="E32" s="10"/>
       <c r="F32" s="10"/>
       <c r="G32" s="11"/>
@@ -2639,19 +2705,19 @@
       <c r="AJ32" s="10"/>
       <c r="AK32" s="10"/>
       <c r="AL32" s="11"/>
-      <c r="AM32" s="43"/>
-      <c r="AN32" s="44"/>
-      <c r="AO32" s="44"/>
-      <c r="AP32" s="44"/>
-      <c r="AQ32" s="44"/>
-      <c r="AR32" s="44"/>
-      <c r="AS32" s="44"/>
-      <c r="AT32" s="45"/>
+      <c r="AM32" s="39"/>
+      <c r="AN32" s="40"/>
+      <c r="AO32" s="40"/>
+      <c r="AP32" s="40"/>
+      <c r="AQ32" s="40"/>
+      <c r="AR32" s="40"/>
+      <c r="AS32" s="40"/>
+      <c r="AT32" s="41"/>
     </row>
     <row r="33" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B33" s="29"/>
-      <c r="C33" s="30"/>
-      <c r="D33" s="31"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="27"/>
       <c r="E33" s="10"/>
       <c r="F33" s="10"/>
       <c r="G33" s="11"/>
@@ -2686,19 +2752,19 @@
       <c r="AJ33" s="10"/>
       <c r="AK33" s="10"/>
       <c r="AL33" s="11"/>
-      <c r="AM33" s="43"/>
-      <c r="AN33" s="44"/>
-      <c r="AO33" s="44"/>
-      <c r="AP33" s="44"/>
-      <c r="AQ33" s="44"/>
-      <c r="AR33" s="44"/>
-      <c r="AS33" s="44"/>
-      <c r="AT33" s="45"/>
+      <c r="AM33" s="39"/>
+      <c r="AN33" s="40"/>
+      <c r="AO33" s="40"/>
+      <c r="AP33" s="40"/>
+      <c r="AQ33" s="40"/>
+      <c r="AR33" s="40"/>
+      <c r="AS33" s="40"/>
+      <c r="AT33" s="41"/>
     </row>
     <row r="34" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B34" s="29"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="31"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="27"/>
       <c r="E34" s="10"/>
       <c r="F34" s="10"/>
       <c r="G34" s="11"/>
@@ -2733,19 +2799,19 @@
       <c r="AJ34" s="10"/>
       <c r="AK34" s="10"/>
       <c r="AL34" s="11"/>
-      <c r="AM34" s="43"/>
-      <c r="AN34" s="44"/>
-      <c r="AO34" s="44"/>
-      <c r="AP34" s="44"/>
-      <c r="AQ34" s="44"/>
-      <c r="AR34" s="44"/>
-      <c r="AS34" s="44"/>
-      <c r="AT34" s="45"/>
+      <c r="AM34" s="39"/>
+      <c r="AN34" s="40"/>
+      <c r="AO34" s="40"/>
+      <c r="AP34" s="40"/>
+      <c r="AQ34" s="40"/>
+      <c r="AR34" s="40"/>
+      <c r="AS34" s="40"/>
+      <c r="AT34" s="41"/>
     </row>
     <row r="35" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B35" s="29"/>
-      <c r="C35" s="30"/>
-      <c r="D35" s="31"/>
+      <c r="B35" s="25"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="27"/>
       <c r="E35" s="10"/>
       <c r="F35" s="10"/>
       <c r="G35" s="11"/>
@@ -2780,19 +2846,19 @@
       <c r="AJ35" s="10"/>
       <c r="AK35" s="10"/>
       <c r="AL35" s="11"/>
-      <c r="AM35" s="43"/>
-      <c r="AN35" s="44"/>
-      <c r="AO35" s="44"/>
-      <c r="AP35" s="44"/>
-      <c r="AQ35" s="44"/>
-      <c r="AR35" s="44"/>
-      <c r="AS35" s="44"/>
-      <c r="AT35" s="45"/>
+      <c r="AM35" s="39"/>
+      <c r="AN35" s="40"/>
+      <c r="AO35" s="40"/>
+      <c r="AP35" s="40"/>
+      <c r="AQ35" s="40"/>
+      <c r="AR35" s="40"/>
+      <c r="AS35" s="40"/>
+      <c r="AT35" s="41"/>
     </row>
     <row r="36" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B36" s="29"/>
-      <c r="C36" s="30"/>
-      <c r="D36" s="31"/>
+      <c r="B36" s="25"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="27"/>
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
       <c r="G36" s="11"/>
@@ -2827,19 +2893,19 @@
       <c r="AJ36" s="10"/>
       <c r="AK36" s="10"/>
       <c r="AL36" s="11"/>
-      <c r="AM36" s="43"/>
-      <c r="AN36" s="44"/>
-      <c r="AO36" s="44"/>
-      <c r="AP36" s="44"/>
-      <c r="AQ36" s="44"/>
-      <c r="AR36" s="44"/>
-      <c r="AS36" s="44"/>
-      <c r="AT36" s="45"/>
+      <c r="AM36" s="39"/>
+      <c r="AN36" s="40"/>
+      <c r="AO36" s="40"/>
+      <c r="AP36" s="40"/>
+      <c r="AQ36" s="40"/>
+      <c r="AR36" s="40"/>
+      <c r="AS36" s="40"/>
+      <c r="AT36" s="41"/>
     </row>
     <row r="37" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B37" s="29"/>
-      <c r="C37" s="30"/>
-      <c r="D37" s="31"/>
+      <c r="B37" s="25"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="27"/>
       <c r="E37" s="10"/>
       <c r="F37" s="10"/>
       <c r="G37" s="11"/>
@@ -2874,19 +2940,19 @@
       <c r="AJ37" s="10"/>
       <c r="AK37" s="10"/>
       <c r="AL37" s="11"/>
-      <c r="AM37" s="43"/>
-      <c r="AN37" s="44"/>
-      <c r="AO37" s="44"/>
-      <c r="AP37" s="44"/>
-      <c r="AQ37" s="44"/>
-      <c r="AR37" s="44"/>
-      <c r="AS37" s="44"/>
-      <c r="AT37" s="45"/>
+      <c r="AM37" s="39"/>
+      <c r="AN37" s="40"/>
+      <c r="AO37" s="40"/>
+      <c r="AP37" s="40"/>
+      <c r="AQ37" s="40"/>
+      <c r="AR37" s="40"/>
+      <c r="AS37" s="40"/>
+      <c r="AT37" s="41"/>
     </row>
     <row r="38" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B38" s="29"/>
-      <c r="C38" s="30"/>
-      <c r="D38" s="31"/>
+      <c r="B38" s="25"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="27"/>
       <c r="E38" s="10"/>
       <c r="F38" s="10"/>
       <c r="G38" s="11"/>
@@ -2921,19 +2987,19 @@
       <c r="AJ38" s="10"/>
       <c r="AK38" s="10"/>
       <c r="AL38" s="11"/>
-      <c r="AM38" s="43"/>
-      <c r="AN38" s="44"/>
-      <c r="AO38" s="44"/>
-      <c r="AP38" s="44"/>
-      <c r="AQ38" s="44"/>
-      <c r="AR38" s="44"/>
-      <c r="AS38" s="44"/>
-      <c r="AT38" s="45"/>
+      <c r="AM38" s="39"/>
+      <c r="AN38" s="40"/>
+      <c r="AO38" s="40"/>
+      <c r="AP38" s="40"/>
+      <c r="AQ38" s="40"/>
+      <c r="AR38" s="40"/>
+      <c r="AS38" s="40"/>
+      <c r="AT38" s="41"/>
     </row>
     <row r="39" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B39" s="29"/>
-      <c r="C39" s="30"/>
-      <c r="D39" s="31"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="27"/>
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
       <c r="G39" s="11"/>
@@ -2968,19 +3034,19 @@
       <c r="AJ39" s="10"/>
       <c r="AK39" s="10"/>
       <c r="AL39" s="11"/>
-      <c r="AM39" s="43"/>
-      <c r="AN39" s="44"/>
-      <c r="AO39" s="44"/>
-      <c r="AP39" s="44"/>
-      <c r="AQ39" s="44"/>
-      <c r="AR39" s="44"/>
-      <c r="AS39" s="44"/>
-      <c r="AT39" s="45"/>
+      <c r="AM39" s="39"/>
+      <c r="AN39" s="40"/>
+      <c r="AO39" s="40"/>
+      <c r="AP39" s="40"/>
+      <c r="AQ39" s="40"/>
+      <c r="AR39" s="40"/>
+      <c r="AS39" s="40"/>
+      <c r="AT39" s="41"/>
     </row>
     <row r="40" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B40" s="29"/>
-      <c r="C40" s="30"/>
-      <c r="D40" s="31"/>
+      <c r="B40" s="25"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="27"/>
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
       <c r="G40" s="11"/>
@@ -3015,19 +3081,19 @@
       <c r="AJ40" s="10"/>
       <c r="AK40" s="10"/>
       <c r="AL40" s="11"/>
-      <c r="AM40" s="43"/>
-      <c r="AN40" s="44"/>
-      <c r="AO40" s="44"/>
-      <c r="AP40" s="44"/>
-      <c r="AQ40" s="44"/>
-      <c r="AR40" s="44"/>
-      <c r="AS40" s="44"/>
-      <c r="AT40" s="45"/>
+      <c r="AM40" s="39"/>
+      <c r="AN40" s="40"/>
+      <c r="AO40" s="40"/>
+      <c r="AP40" s="40"/>
+      <c r="AQ40" s="40"/>
+      <c r="AR40" s="40"/>
+      <c r="AS40" s="40"/>
+      <c r="AT40" s="41"/>
     </row>
     <row r="41" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B41" s="29"/>
-      <c r="C41" s="30"/>
-      <c r="D41" s="31"/>
+      <c r="B41" s="25"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="27"/>
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
       <c r="G41" s="11"/>
@@ -3062,19 +3128,19 @@
       <c r="AJ41" s="10"/>
       <c r="AK41" s="10"/>
       <c r="AL41" s="11"/>
-      <c r="AM41" s="43"/>
-      <c r="AN41" s="44"/>
-      <c r="AO41" s="44"/>
-      <c r="AP41" s="44"/>
-      <c r="AQ41" s="44"/>
-      <c r="AR41" s="44"/>
-      <c r="AS41" s="44"/>
-      <c r="AT41" s="45"/>
+      <c r="AM41" s="39"/>
+      <c r="AN41" s="40"/>
+      <c r="AO41" s="40"/>
+      <c r="AP41" s="40"/>
+      <c r="AQ41" s="40"/>
+      <c r="AR41" s="40"/>
+      <c r="AS41" s="40"/>
+      <c r="AT41" s="41"/>
     </row>
     <row r="42" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B42" s="29"/>
-      <c r="C42" s="30"/>
-      <c r="D42" s="31"/>
+      <c r="B42" s="25"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="27"/>
       <c r="E42" s="10"/>
       <c r="F42" s="10"/>
       <c r="G42" s="11"/>
@@ -3109,19 +3175,19 @@
       <c r="AJ42" s="10"/>
       <c r="AK42" s="10"/>
       <c r="AL42" s="11"/>
-      <c r="AM42" s="43"/>
-      <c r="AN42" s="44"/>
-      <c r="AO42" s="44"/>
-      <c r="AP42" s="44"/>
-      <c r="AQ42" s="44"/>
-      <c r="AR42" s="44"/>
-      <c r="AS42" s="44"/>
-      <c r="AT42" s="45"/>
+      <c r="AM42" s="39"/>
+      <c r="AN42" s="40"/>
+      <c r="AO42" s="40"/>
+      <c r="AP42" s="40"/>
+      <c r="AQ42" s="40"/>
+      <c r="AR42" s="40"/>
+      <c r="AS42" s="40"/>
+      <c r="AT42" s="41"/>
     </row>
     <row r="43" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B43" s="29"/>
-      <c r="C43" s="30"/>
-      <c r="D43" s="31"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="27"/>
       <c r="E43" s="10"/>
       <c r="F43" s="10"/>
       <c r="G43" s="11"/>
@@ -3156,19 +3222,19 @@
       <c r="AJ43" s="10"/>
       <c r="AK43" s="10"/>
       <c r="AL43" s="11"/>
-      <c r="AM43" s="43"/>
-      <c r="AN43" s="44"/>
-      <c r="AO43" s="44"/>
-      <c r="AP43" s="44"/>
-      <c r="AQ43" s="44"/>
-      <c r="AR43" s="44"/>
-      <c r="AS43" s="44"/>
-      <c r="AT43" s="45"/>
+      <c r="AM43" s="39"/>
+      <c r="AN43" s="40"/>
+      <c r="AO43" s="40"/>
+      <c r="AP43" s="40"/>
+      <c r="AQ43" s="40"/>
+      <c r="AR43" s="40"/>
+      <c r="AS43" s="40"/>
+      <c r="AT43" s="41"/>
     </row>
     <row r="44" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B44" s="29"/>
-      <c r="C44" s="30"/>
-      <c r="D44" s="31"/>
+      <c r="B44" s="25"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="27"/>
       <c r="E44" s="10"/>
       <c r="F44" s="10"/>
       <c r="G44" s="11"/>
@@ -3203,19 +3269,19 @@
       <c r="AJ44" s="10"/>
       <c r="AK44" s="10"/>
       <c r="AL44" s="11"/>
-      <c r="AM44" s="43"/>
-      <c r="AN44" s="44"/>
-      <c r="AO44" s="44"/>
-      <c r="AP44" s="44"/>
-      <c r="AQ44" s="44"/>
-      <c r="AR44" s="44"/>
-      <c r="AS44" s="44"/>
-      <c r="AT44" s="45"/>
+      <c r="AM44" s="39"/>
+      <c r="AN44" s="40"/>
+      <c r="AO44" s="40"/>
+      <c r="AP44" s="40"/>
+      <c r="AQ44" s="40"/>
+      <c r="AR44" s="40"/>
+      <c r="AS44" s="40"/>
+      <c r="AT44" s="41"/>
     </row>
     <row r="45" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B45" s="29"/>
-      <c r="C45" s="30"/>
-      <c r="D45" s="31"/>
+      <c r="B45" s="25"/>
+      <c r="C45" s="26"/>
+      <c r="D45" s="27"/>
       <c r="E45" s="10"/>
       <c r="F45" s="10"/>
       <c r="G45" s="11"/>
@@ -3250,19 +3316,19 @@
       <c r="AJ45" s="10"/>
       <c r="AK45" s="10"/>
       <c r="AL45" s="11"/>
-      <c r="AM45" s="43"/>
-      <c r="AN45" s="44"/>
-      <c r="AO45" s="44"/>
-      <c r="AP45" s="44"/>
-      <c r="AQ45" s="44"/>
-      <c r="AR45" s="44"/>
-      <c r="AS45" s="44"/>
-      <c r="AT45" s="45"/>
+      <c r="AM45" s="39"/>
+      <c r="AN45" s="40"/>
+      <c r="AO45" s="40"/>
+      <c r="AP45" s="40"/>
+      <c r="AQ45" s="40"/>
+      <c r="AR45" s="40"/>
+      <c r="AS45" s="40"/>
+      <c r="AT45" s="41"/>
     </row>
     <row r="46" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B46" s="29"/>
-      <c r="C46" s="30"/>
-      <c r="D46" s="31"/>
+      <c r="B46" s="25"/>
+      <c r="C46" s="26"/>
+      <c r="D46" s="27"/>
       <c r="E46" s="10"/>
       <c r="F46" s="10"/>
       <c r="G46" s="11"/>
@@ -3297,19 +3363,19 @@
       <c r="AJ46" s="10"/>
       <c r="AK46" s="10"/>
       <c r="AL46" s="11"/>
-      <c r="AM46" s="43"/>
-      <c r="AN46" s="44"/>
-      <c r="AO46" s="44"/>
-      <c r="AP46" s="44"/>
-      <c r="AQ46" s="44"/>
-      <c r="AR46" s="44"/>
-      <c r="AS46" s="44"/>
-      <c r="AT46" s="45"/>
+      <c r="AM46" s="39"/>
+      <c r="AN46" s="40"/>
+      <c r="AO46" s="40"/>
+      <c r="AP46" s="40"/>
+      <c r="AQ46" s="40"/>
+      <c r="AR46" s="40"/>
+      <c r="AS46" s="40"/>
+      <c r="AT46" s="41"/>
     </row>
     <row r="47" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B47" s="29"/>
-      <c r="C47" s="30"/>
-      <c r="D47" s="31"/>
+      <c r="B47" s="25"/>
+      <c r="C47" s="26"/>
+      <c r="D47" s="27"/>
       <c r="E47" s="10"/>
       <c r="F47" s="10"/>
       <c r="G47" s="11"/>
@@ -3344,19 +3410,19 @@
       <c r="AJ47" s="10"/>
       <c r="AK47" s="10"/>
       <c r="AL47" s="11"/>
-      <c r="AM47" s="43"/>
-      <c r="AN47" s="44"/>
-      <c r="AO47" s="44"/>
-      <c r="AP47" s="44"/>
-      <c r="AQ47" s="44"/>
-      <c r="AR47" s="44"/>
-      <c r="AS47" s="44"/>
-      <c r="AT47" s="45"/>
+      <c r="AM47" s="39"/>
+      <c r="AN47" s="40"/>
+      <c r="AO47" s="40"/>
+      <c r="AP47" s="40"/>
+      <c r="AQ47" s="40"/>
+      <c r="AR47" s="40"/>
+      <c r="AS47" s="40"/>
+      <c r="AT47" s="41"/>
     </row>
     <row r="48" spans="2:46" x14ac:dyDescent="0.25">
-      <c r="B48" s="29"/>
-      <c r="C48" s="30"/>
-      <c r="D48" s="31"/>
+      <c r="B48" s="25"/>
+      <c r="C48" s="26"/>
+      <c r="D48" s="27"/>
       <c r="E48" s="10"/>
       <c r="F48" s="10"/>
       <c r="G48" s="11"/>
@@ -3391,19 +3457,19 @@
       <c r="AJ48" s="10"/>
       <c r="AK48" s="10"/>
       <c r="AL48" s="11"/>
-      <c r="AM48" s="43"/>
-      <c r="AN48" s="44"/>
-      <c r="AO48" s="44"/>
-      <c r="AP48" s="44"/>
-      <c r="AQ48" s="44"/>
-      <c r="AR48" s="44"/>
-      <c r="AS48" s="44"/>
-      <c r="AT48" s="45"/>
+      <c r="AM48" s="39"/>
+      <c r="AN48" s="40"/>
+      <c r="AO48" s="40"/>
+      <c r="AP48" s="40"/>
+      <c r="AQ48" s="40"/>
+      <c r="AR48" s="40"/>
+      <c r="AS48" s="40"/>
+      <c r="AT48" s="41"/>
     </row>
     <row r="49" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="B49" s="29"/>
-      <c r="C49" s="30"/>
-      <c r="D49" s="31"/>
+      <c r="B49" s="25"/>
+      <c r="C49" s="26"/>
+      <c r="D49" s="27"/>
       <c r="E49" s="10"/>
       <c r="F49" s="10"/>
       <c r="G49" s="11"/>
@@ -3438,26 +3504,26 @@
       <c r="AJ49" s="10"/>
       <c r="AK49" s="10"/>
       <c r="AL49" s="11"/>
-      <c r="AM49" s="43"/>
-      <c r="AN49" s="44"/>
-      <c r="AO49" s="44"/>
-      <c r="AP49" s="44"/>
-      <c r="AQ49" s="44"/>
-      <c r="AR49" s="44"/>
-      <c r="AS49" s="44"/>
-      <c r="AT49" s="45"/>
+      <c r="AM49" s="39"/>
+      <c r="AN49" s="40"/>
+      <c r="AO49" s="40"/>
+      <c r="AP49" s="40"/>
+      <c r="AQ49" s="40"/>
+      <c r="AR49" s="40"/>
+      <c r="AS49" s="40"/>
+      <c r="AT49" s="41"/>
     </row>
     <row r="50" spans="1:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>5</v>
       </c>
-      <c r="B50" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="C50" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="D50" s="34" t="s">
+      <c r="B50" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" s="30" t="s">
         <v>5</v>
       </c>
       <c r="E50" s="13" t="s">
@@ -3562,28 +3628,28 @@
       <c r="AL50" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="AM50" s="46" t="s">
-        <v>5</v>
-      </c>
-      <c r="AN50" s="47" t="s">
-        <v>5</v>
-      </c>
-      <c r="AO50" s="47" t="s">
-        <v>5</v>
-      </c>
-      <c r="AP50" s="47" t="s">
-        <v>5</v>
-      </c>
-      <c r="AQ50" s="47" t="s">
-        <v>5</v>
-      </c>
-      <c r="AR50" s="47" t="s">
-        <v>5</v>
-      </c>
-      <c r="AS50" s="47" t="s">
-        <v>5</v>
-      </c>
-      <c r="AT50" s="48" t="s">
+      <c r="AM50" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN50" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="AO50" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="AP50" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="AQ50" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="AR50" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="AS50" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="AT50" s="44" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3600,185 +3666,1150 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C13:C46"/>
+  <dimension ref="A1:AN50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:C46"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="3.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.7109375" style="10" customWidth="1"/>
+    <col min="12" max="12" width="3.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.7109375" style="10" customWidth="1"/>
+    <col min="14" max="18" width="3.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="3.7109375" style="10" customWidth="1"/>
+    <col min="21" max="39" width="3.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="6.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="41" max="16384" width="10.140625" style="10"/>
+  </cols>
   <sheetData>
-    <row r="13" spans="3:3" ht="27.75" x14ac:dyDescent="0.25">
-      <c r="C13" s="7" t="s">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="66" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
+      <c r="L1" s="66"/>
+      <c r="M1" s="66"/>
+      <c r="N1" s="66"/>
+      <c r="O1" s="66"/>
+      <c r="P1" s="66"/>
+      <c r="Q1" s="66"/>
+      <c r="R1" s="66"/>
+      <c r="S1" s="66"/>
+      <c r="T1" s="66"/>
+      <c r="U1" s="66"/>
+      <c r="V1" s="66"/>
+      <c r="W1" s="66"/>
+      <c r="X1" s="66"/>
+      <c r="Y1" s="66"/>
+      <c r="Z1" s="66"/>
+      <c r="AA1" s="66"/>
+      <c r="AB1" s="66"/>
+      <c r="AC1" s="66"/>
+      <c r="AD1" s="66"/>
+      <c r="AE1" s="66"/>
+      <c r="AF1" s="66"/>
+      <c r="AG1" s="66"/>
+      <c r="AH1" s="66"/>
+      <c r="AI1" s="66"/>
+      <c r="AJ1" s="66"/>
+      <c r="AK1" s="66"/>
+      <c r="AL1" s="66"/>
+      <c r="AM1" s="66"/>
+      <c r="AN1" s="67" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" s="55" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="B2" s="56" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="56" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="56" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="56" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="56" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="56" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" s="56" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="56" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" s="56" t="s">
+        <v>47</v>
+      </c>
+      <c r="M2" s="56" t="s">
+        <v>47</v>
+      </c>
+      <c r="N2" s="56" t="s">
+        <v>47</v>
+      </c>
+      <c r="O2" s="56" t="s">
+        <v>47</v>
+      </c>
+      <c r="P2" s="56" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q2" s="56" t="s">
+        <v>47</v>
+      </c>
+      <c r="R2" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="S2" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="T2" s="56" t="s">
+        <v>11</v>
+      </c>
+      <c r="U2" s="56" t="s">
+        <v>48</v>
+      </c>
+      <c r="V2" s="56" t="s">
+        <v>48</v>
+      </c>
+      <c r="W2" s="56" t="s">
+        <v>48</v>
+      </c>
+      <c r="X2" s="56" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y2" s="56" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z2" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA2" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB2" s="56" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC2" s="56" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD2" s="56" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE2" s="56" t="s">
+        <v>53</v>
+      </c>
+      <c r="AF2" s="56" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG2" s="56" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH2" s="56" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI2" s="56" t="s">
+        <v>54</v>
+      </c>
+      <c r="AJ2" s="56" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK2" s="56" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL2" s="56" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM2" s="56" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN2" s="67"/>
+    </row>
+    <row r="3" spans="1:40" s="7" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="3:3" ht="21.75" x14ac:dyDescent="0.25">
-      <c r="C14" s="7" t="s">
+      <c r="C3" s="7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="3:3" ht="29.25" x14ac:dyDescent="0.25">
-      <c r="C15" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="3:3" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="C16" s="6" t="s">
+      <c r="E3" s="7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="3:3" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="C17" s="8" t="s">
+      <c r="F3" s="7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="3:3" ht="41.25" x14ac:dyDescent="0.25">
-      <c r="C18" s="6" t="s">
+      <c r="G3" s="7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="3:3" ht="48" x14ac:dyDescent="0.25">
-      <c r="C19" s="8" t="s">
+      <c r="H3" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="20" spans="3:3" ht="46.5" x14ac:dyDescent="0.25">
-      <c r="C20" s="6" t="s">
+      <c r="I3" s="7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="21" spans="3:3" ht="53.25" x14ac:dyDescent="0.25">
-      <c r="C21" s="8" t="s">
+      <c r="J3" s="7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="22" spans="3:3" ht="21.75" x14ac:dyDescent="0.25">
-      <c r="C22" s="6" t="s">
+      <c r="K3" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="L3" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="23" spans="3:3" ht="21.75" x14ac:dyDescent="0.25">
-      <c r="C23" s="7" t="s">
+      <c r="M3" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="N3" s="7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="24" spans="3:3" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="C24" s="7" t="s">
+      <c r="O3" s="7" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="25" spans="3:3" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="C25" s="7" t="s">
+      <c r="P3" s="7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="26" spans="3:3" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="C26" s="8" t="s">
+      <c r="Q3" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="27" spans="3:3" ht="30.75" x14ac:dyDescent="0.25">
-      <c r="C27" s="16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="3:3" ht="24" x14ac:dyDescent="0.25">
-      <c r="C28" s="6" t="s">
+      <c r="R3" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="S3" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="T3" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="U3" s="7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="29" spans="3:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="C29" s="7" t="s">
+      <c r="V3" s="7" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="30" spans="3:3" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="C30" s="7" t="s">
+      <c r="W3" s="7" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="31" spans="3:3" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="C31" s="7" t="s">
+      <c r="X3" s="7" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="32" spans="3:3" ht="24" x14ac:dyDescent="0.25">
-      <c r="C32" s="8" t="s">
+      <c r="Y3" s="7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="33" spans="3:3" ht="27" x14ac:dyDescent="0.25">
-      <c r="C33" s="6" t="s">
+      <c r="Z3" s="7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="34" spans="3:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C34" s="8" t="s">
+      <c r="AA3" s="7" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="35" spans="3:3" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="C35" s="16" t="s">
+      <c r="AB3" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="36" spans="3:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="C36" s="6" t="s">
+      <c r="AC3" s="7" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="37" spans="3:3" ht="24" x14ac:dyDescent="0.25">
-      <c r="C37" s="8" t="s">
+      <c r="AD3" s="7" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="38" spans="3:3" ht="30.75" x14ac:dyDescent="0.25">
-      <c r="C38" s="16" t="s">
+      <c r="AE3" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="39" spans="3:3" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="C39" s="6" t="s">
+      <c r="AF3" s="7" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="3:3" ht="32.25" x14ac:dyDescent="0.25">
-      <c r="C40" s="8" t="s">
+      <c r="AG3" s="7" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="3:3" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="C41" s="6" t="s">
+      <c r="AH3" s="7" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="3:3" ht="21.75" x14ac:dyDescent="0.25">
-      <c r="C42" s="7" t="s">
+      <c r="AI3" s="7" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="43" spans="3:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="C43" s="7" t="s">
+      <c r="AJ3" s="7" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="44" spans="3:3" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="C44" s="7" t="s">
+      <c r="AK3" s="7" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="45" spans="3:3" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="C45" s="7" t="s">
+      <c r="AL3" s="7" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="3:3" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="C46" s="8" t="s">
+      <c r="AM3" s="7" t="s">
         <v>45</v>
       </c>
+      <c r="AN3" s="67"/>
+    </row>
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A4" s="58" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="60"/>
+      <c r="G4" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="61"/>
+      <c r="L4" s="61"/>
+      <c r="M4" s="61"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="P4" s="61"/>
+      <c r="Q4" s="61"/>
+      <c r="R4" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="S4" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="T4" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="U4" s="61"/>
+      <c r="V4" s="61"/>
+      <c r="W4" s="61"/>
+      <c r="X4" s="61"/>
+      <c r="Y4" s="61"/>
+      <c r="Z4" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA4" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB4" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC4" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD4" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE4" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF4" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG4" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH4" s="61"/>
+      <c r="AI4" s="61"/>
+      <c r="AJ4" s="61"/>
+      <c r="AK4" s="61"/>
+      <c r="AL4" s="61"/>
+      <c r="AM4" s="61"/>
+      <c r="AN4" s="26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A5" s="58" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="61"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
+      <c r="G5" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="K5" s="61"/>
+      <c r="L5" s="61"/>
+      <c r="M5" s="61"/>
+      <c r="N5" s="61"/>
+      <c r="O5" s="61"/>
+      <c r="P5" s="61"/>
+      <c r="Q5" s="61"/>
+      <c r="R5" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="S5" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="T5" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="U5" s="61"/>
+      <c r="V5" s="61"/>
+      <c r="W5" s="61"/>
+      <c r="X5" s="61"/>
+      <c r="Y5" s="61"/>
+      <c r="Z5" s="60"/>
+      <c r="AA5" s="61"/>
+      <c r="AB5" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC5" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD5" s="61"/>
+      <c r="AE5" s="60"/>
+      <c r="AF5" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG5" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH5" s="61"/>
+      <c r="AI5" s="61"/>
+      <c r="AJ5" s="61"/>
+      <c r="AK5" s="61"/>
+      <c r="AL5" s="61"/>
+      <c r="AM5" s="61"/>
+      <c r="AN5" s="26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A6" s="58" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="60"/>
+      <c r="G6" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="K6" s="61"/>
+      <c r="L6" s="61"/>
+      <c r="M6" s="61"/>
+      <c r="N6" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="O6" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="P6" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q6" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="R6" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="S6" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="T6" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="U6" s="61"/>
+      <c r="V6" s="61"/>
+      <c r="W6" s="61"/>
+      <c r="X6" s="61"/>
+      <c r="Y6" s="61"/>
+      <c r="Z6" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA6" s="60"/>
+      <c r="AB6" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC6" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD6" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE6" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF6" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG6" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH6" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI6" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AJ6" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK6" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AL6" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM6" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN6" s="26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A7" s="58" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="60"/>
+      <c r="G7" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="J7" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="K7" s="61"/>
+      <c r="L7" s="61"/>
+      <c r="M7" s="61"/>
+      <c r="N7" s="61"/>
+      <c r="O7" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="P7" s="61"/>
+      <c r="Q7" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="R7" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="S7" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="T7" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="U7" s="61"/>
+      <c r="V7" s="61"/>
+      <c r="W7" s="61"/>
+      <c r="X7" s="61"/>
+      <c r="Y7" s="61"/>
+      <c r="Z7" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA7" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB7" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC7" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD7" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE7" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF7" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG7" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH7" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI7" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AJ7" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK7" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AL7" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM7" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN7" s="26" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A8" s="58" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="60"/>
+      <c r="G8" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="J8" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="K8" s="61"/>
+      <c r="L8" s="61"/>
+      <c r="M8" s="61"/>
+      <c r="N8" s="61"/>
+      <c r="O8" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="P8" s="61"/>
+      <c r="Q8" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="R8" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="S8" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="T8" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="U8" s="61"/>
+      <c r="V8" s="61"/>
+      <c r="W8" s="61"/>
+      <c r="X8" s="61"/>
+      <c r="Y8" s="61"/>
+      <c r="Z8" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA8" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB8" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC8" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD8" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE8" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF8" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG8" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH8" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI8" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AJ8" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK8" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AL8" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM8" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN8" s="57" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A9" s="58" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="61"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="60"/>
+      <c r="G9" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="H9" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="J9" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="K9" s="61"/>
+      <c r="L9" s="61"/>
+      <c r="M9" s="61"/>
+      <c r="N9" s="61"/>
+      <c r="O9" s="61"/>
+      <c r="P9" s="61"/>
+      <c r="Q9" s="61"/>
+      <c r="R9" s="61"/>
+      <c r="S9" s="61"/>
+      <c r="T9" s="61"/>
+      <c r="U9" s="61"/>
+      <c r="V9" s="61"/>
+      <c r="W9" s="61"/>
+      <c r="X9" s="61"/>
+      <c r="Y9" s="61"/>
+      <c r="Z9" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA9" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB9" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC9" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD9" s="61"/>
+      <c r="AE9" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF9" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG9" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH9" s="61"/>
+      <c r="AI9" s="61"/>
+      <c r="AJ9" s="61"/>
+      <c r="AK9" s="61"/>
+      <c r="AL9" s="61"/>
+      <c r="AM9" s="61"/>
+      <c r="AN9" s="57" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A10" s="58" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="60"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="J10" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="K10" s="61"/>
+      <c r="L10" s="61"/>
+      <c r="M10" s="61"/>
+      <c r="N10" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="O10" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="P10" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q10" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="R10" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="S10" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="T10" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="U10" s="61"/>
+      <c r="V10" s="61"/>
+      <c r="W10" s="61"/>
+      <c r="X10" s="61"/>
+      <c r="Y10" s="61"/>
+      <c r="Z10" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA10" s="60"/>
+      <c r="AB10" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC10" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD10" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE10" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF10" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG10" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH10" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI10" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AJ10" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK10" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AL10" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM10" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN10" s="26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A11" s="58" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="60"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="J11" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="K11" s="61"/>
+      <c r="L11" s="61"/>
+      <c r="M11" s="61"/>
+      <c r="N11" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="O11" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="P11" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q11" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="R11" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="S11" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="T11" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="U11" s="61"/>
+      <c r="V11" s="61"/>
+      <c r="W11" s="61"/>
+      <c r="X11" s="61"/>
+      <c r="Y11" s="61"/>
+      <c r="Z11" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA11" s="60"/>
+      <c r="AB11" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC11" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD11" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE11" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF11" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG11" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH11" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI11" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AJ11" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK11" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AL11" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM11" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN11" s="26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="50" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A50" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E50" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F50" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G50" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H50" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I50" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="J50" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="L50" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="N50" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="O50" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="P50" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q50" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="R50" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="U50" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="V50" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="W50" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="X50" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y50" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z50" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA50" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB50" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC50" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD50" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE50" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF50" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG50" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH50" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI50" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="AJ50" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK50" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="AL50" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM50" s="10" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:AM1"/>
+    <mergeCell ref="AN1:AN3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="U2:AM2 B2:Q2 R2:T2" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>